<commit_message>
finally understood linkedlist! and completed a easy qn on leetcode
</commit_message>
<xml_diff>
--- a/LeetCode/Compiled.xlsx
+++ b/LeetCode/Compiled.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiji\Documents\GitHub\learning_java\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811CB35E-8121-47D4-B867-2B75474159FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0352EF48-87E1-4FB7-9D08-95B058890C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{76B0388C-7AFC-4A8E-8947-BAD2CE830851}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Question</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Using stacks; push the opening bracket first if the next is not the respective closing bracket. If it is, pop.</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>Using linkedlists concept, compare node values.</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,9 +496,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
attempted one leetcode qn
</commit_message>
<xml_diff>
--- a/LeetCode/Compiled.xlsx
+++ b/LeetCode/Compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiji\Documents\GitHub\learning_java\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0352EF48-87E1-4FB7-9D08-95B058890C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD58FA62-4777-4FF9-AA43-54C1DD2977B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{76B0388C-7AFC-4A8E-8947-BAD2CE830851}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Question</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Using linkedlists concept, compare node values.</t>
+  </si>
+  <si>
+    <t>Maximum SubArray</t>
+  </si>
+  <si>
+    <t>Kadane's algorithm. Loop through once, if the currentSum &lt; 0 initialize back to 0. need to self check cause sometimes it may not be less than 0 but can be smaller than previous combination</t>
   </si>
 </sst>
 </file>
@@ -450,17 +456,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C471E23E-69C8-4741-AAAB-5BFCBE85727A}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="92.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="154.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -474,7 +480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -485,7 +491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -496,7 +502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -507,46 +513,89 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
+    <row r="15" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>